<commit_message>
Fixed a small error with the MonRegisterInterpreter
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Skrivbord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38158FC5-8462-45CA-9026-DD1A47B88C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A0B7BD-9090-48D9-938A-A7CEA2C36DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="1545" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
+    <workbookView xWindow="32505" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,6 @@
     <t>Bulbasuar</t>
   </si>
   <si>
-    <t>Grass</t>
-  </si>
-  <si>
-    <t>Poison</t>
-  </si>
-  <si>
     <t>base attack</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>Tauros</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>Rasmusmon</t>
   </si>
   <si>
@@ -97,6 +88,15 @@
   </si>
   <si>
     <t>evolution id</t>
+  </si>
+  <si>
+    <t>GRASS</t>
+  </si>
+  <si>
+    <t>NORMAL</t>
+  </si>
+  <si>
+    <t>POISON</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -479,22 +479,22 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
@@ -514,10 +514,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>45</v>
@@ -543,13 +543,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>60</v>
@@ -575,13 +575,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>80</v>
@@ -607,10 +607,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>75</v>
@@ -636,7 +636,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -645,18 +645,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -831,14 +831,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -851,6 +843,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added attacks to Puckemon
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/Documents/GitHub/bEsTpRoGrAmMerS_EU/src/main/java/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A0B7BD-9090-48D9-938A-A7CEA2C36DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB2B28F-2BBB-314D-B72A-8F8A17ED3BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32505" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>POISON</t>
+  </si>
+  <si>
+    <t>Tackle,SwordsDance</t>
   </si>
 </sst>
 </file>
@@ -132,8 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,21 +457,21 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -506,7 +512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -537,8 +543,11 @@
       <c r="J2">
         <v>2</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -570,7 +579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -602,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -631,7 +640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Created the PuckebagScreen to be used during combat. Added the assets for it. Wrote the code to make it render the current party Puckemon.
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmilJonsson\Documents\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A493BAFD-7DD4-4798-8FEB-96CD08A235C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85146438-818D-447B-9341-1F020F9B0E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -454,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB97F33-6489-4E92-9DBD-0E2293FD6E3B}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K113" sqref="K113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,41 +617,51 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5">
-        <v>75</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5">
-        <v>95</v>
-      </c>
-      <c r="H5">
-        <v>110</v>
-      </c>
-      <c r="I5">
-        <v>101</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="1"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129" t="s">
+        <v>19</v>
+      </c>
+      <c r="D129" t="s">
+        <v>19</v>
+      </c>
+      <c r="E129">
+        <v>75</v>
+      </c>
+      <c r="F129">
+        <v>100</v>
+      </c>
+      <c r="G129">
+        <v>95</v>
+      </c>
+      <c r="H129">
+        <v>110</v>
+      </c>
+      <c r="I129">
+        <v>101</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+      <c r="L129" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -660,18 +670,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -846,6 +856,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -858,14 +876,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Can now switch Puckemon during Combat. Fixed a bug with Puckemon Stats. Removed the rectangle assets, the program now draws them. The Party shows if a puckemon is unable to battle.
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85146438-818D-447B-9341-1F020F9B0E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589DB69D-4D65-4ADD-9A8A-6EF2C67D771B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>Bulbasuar</t>
-  </si>
-  <si>
     <t>base attack</t>
   </si>
   <si>
@@ -100,6 +97,12 @@
   </si>
   <si>
     <t>Tackle,SwordsDance</t>
+  </si>
+  <si>
+    <t>Bulbasaur</t>
+  </si>
+  <si>
+    <t>Tackle,SwordsDance,Absorb</t>
   </si>
 </sst>
 </file>
@@ -456,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB97F33-6489-4E92-9DBD-0E2293FD6E3B}">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K113" sqref="K113"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +476,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -485,22 +488,22 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
@@ -517,13 +520,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>45</v>
@@ -544,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -552,13 +555,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>60</v>
@@ -579,7 +582,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -587,13 +590,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>80</v>
@@ -614,7 +617,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -622,7 +625,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -634,13 +637,13 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C129" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D129" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E129">
         <v>75</v>
@@ -661,7 +664,7 @@
         <v>0</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -670,18 +673,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -856,14 +859,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -876,6 +871,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Improved on the code ;)
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589DB69D-4D65-4ADD-9A8A-6EF2C67D771B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0820F4-8485-44EE-ABEC-254E962C74A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
+    <workbookView xWindow="3675" yWindow="2145" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Tackle,SwordsDance,Absorb</t>
+  </si>
+  <si>
+    <t>Tackle,SwordsDance,Absorb,QuickAttack,DoubleEdge</t>
   </si>
 </sst>
 </file>
@@ -459,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB97F33-6489-4E92-9DBD-0E2293FD6E3B}">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O120" sqref="O120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +667,7 @@
         <v>0</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some issues with stats and damage calculations. Made it so that you have to switch, cant pick fainted Puckemon.
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0820F4-8485-44EE-ABEC-254E962C74A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2610EA53-C397-4E1B-938B-FB565F743B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="2145" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
+    <workbookView xWindow="32355" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
     <t>Tackle,SwordsDance,Absorb</t>
   </si>
   <si>
-    <t>Tackle,SwordsDance,Absorb,QuickAttack,DoubleEdge</t>
+    <t>Tackle,SwordsDance,QuickAttack,DoubleEdge</t>
   </si>
 </sst>
 </file>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB97F33-6489-4E92-9DBD-0E2293FD6E3B}">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O120" sqref="O120"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L130" sqref="L130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,18 +676,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -862,6 +862,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -874,14 +882,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Did major refractoring to how Puckemon are created. CreatePuckemon now creates them Owned/Wild. Type/s are now a list of 2 enums instead of 2 seperate enums. Solved a bug with the ExcelReader. Tests do need to be remade.
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2610EA53-C397-4E1B-938B-FB565F743B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF5CCD-768B-4AFF-9F10-DBCBC80EDCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32355" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>type 1</t>
-  </si>
-  <si>
-    <t>type 2</t>
-  </si>
-  <si>
     <t>move list</t>
   </si>
   <si>
@@ -87,15 +81,9 @@
     <t>evolution id</t>
   </si>
   <si>
-    <t>GRASS</t>
-  </si>
-  <si>
     <t>NORMAL</t>
   </si>
   <si>
-    <t>POISON</t>
-  </si>
-  <si>
     <t>Tackle,SwordsDance</t>
   </si>
   <si>
@@ -106,6 +94,12 @@
   </si>
   <si>
     <t>Tackle,SwordsDance,QuickAttack,DoubleEdge</t>
+  </si>
+  <si>
+    <t>type/s</t>
+  </si>
+  <si>
+    <t>GRASS, POISON</t>
   </si>
 </sst>
 </file>
@@ -462,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB97F33-6489-4E92-9DBD-0E2293FD6E3B}">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L130" sqref="L130"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,43 +473,40 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -523,34 +514,31 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
+      <c r="D2">
+        <v>45</v>
       </c>
       <c r="E2">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F2">
         <v>49</v>
       </c>
       <c r="G2">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H2">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -558,34 +546,31 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>60</v>
       </c>
       <c r="E3">
+        <v>62</v>
+      </c>
+      <c r="F3">
+        <v>63</v>
+      </c>
+      <c r="G3">
         <v>60</v>
       </c>
-      <c r="F3">
-        <v>62</v>
-      </c>
-      <c r="G3">
-        <v>63</v>
-      </c>
       <c r="H3">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="I3">
-        <v>36</v>
-      </c>
-      <c r="J3">
         <v>3</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>20</v>
+      <c r="K3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -593,34 +578,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>80</v>
       </c>
       <c r="E4">
+        <v>82</v>
+      </c>
+      <c r="F4">
+        <v>83</v>
+      </c>
+      <c r="G4">
         <v>80</v>
       </c>
-      <c r="F4">
-        <v>82</v>
-      </c>
-      <c r="G4">
-        <v>83</v>
-      </c>
       <c r="H4">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="I4">
-        <v>101</v>
-      </c>
-      <c r="J4">
         <v>0</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>22</v>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -628,46 +610,43 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L7" s="1"/>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C129" t="s">
-        <v>18</v>
-      </c>
-      <c r="D129" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="D129">
+        <v>75</v>
       </c>
       <c r="E129">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="F129">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G129">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="H129">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="I129">
-        <v>101</v>
-      </c>
-      <c r="J129">
         <v>0</v>
       </c>
-      <c r="L129" s="1" t="s">
-        <v>23</v>
+      <c r="K129" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -676,18 +655,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -862,14 +841,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -882,6 +853,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed some glitches around the code, started on the evolve method
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BF5CCD-768B-4AFF-9F10-DBCBC80EDCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4D891F-9457-48F5-A45F-4F94A3F6BD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32355" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
+    <workbookView xWindow="4275" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>GRASS, POISON</t>
+  </si>
+  <si>
+    <t>FIRE</t>
+  </si>
+  <si>
+    <t>QuickAttack,Absorb,SwordsDance,Flamethrower</t>
   </si>
 </sst>
 </file>
@@ -457,7 +463,7 @@
   <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +617,30 @@
       </c>
       <c r="B6" t="s">
         <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>50</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>101</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="L6" s="1"/>
     </row>

</xml_diff>

<commit_message>
Model does not create Puckemon any longer, GameBuilder creates all that
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/Documents/GitHub/bEsTpRoGrAmMerS_EU/src/main/java/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C4D891F-9457-48F5-A45F-4F94A3F6BD4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F9F962-2A42-814F-9C53-41FA861DA6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
+    <workbookView xWindow="4280" yWindow="2020" windowWidth="21600" windowHeight="11380" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>QuickAttack,Absorb,SwordsDance,Flamethrower</t>
+  </si>
+  <si>
+    <t>Emilmon</t>
+  </si>
+  <si>
+    <t>Tackle</t>
   </si>
 </sst>
 </file>
@@ -463,21 +469,21 @@
   <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -515,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -547,7 +553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -579,7 +585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -611,7 +617,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>40</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -644,10 +682,10 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L7" s="1"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -685,21 +723,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006124A3112A30234887B80C625186D901" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56c14a6dcb6c84885f089c610ccd3af4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3b6923cc-94d7-4f86-8e31-1b1fa90ab430" xmlns:ns4="79f744f5-cb0c-47fc-b303-4456a0d04880" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efe903cb1c03997b8902cfab651c05c0" ns3:_="" ns4:_="">
     <xsd:import namespace="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
@@ -870,32 +893,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="79f744f5-cb0c-47fc-b303-4456a0d04880"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30B054E4-AB9F-40CB-9C81-093D24B21832}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -912,4 +925,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="79f744f5-cb0c-47fc-b303-4456a0d04880"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PuckeBag have been split in two. VildBag and Playerbag. Fixed some small errors. Added an evolution method.
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/Documents/GitHub/bEsTpRoGrAmMerS_EU/src/main/java/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F9F962-2A42-814F-9C53-41FA861DA6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9F938B-CBF5-D047-9D81-AB070F70CD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4280" yWindow="2020" windowWidth="21600" windowHeight="11380" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:M129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -723,6 +723,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006124A3112A30234887B80C625186D901" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56c14a6dcb6c84885f089c610ccd3af4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3b6923cc-94d7-4f86-8e31-1b1fa90ab430" xmlns:ns4="79f744f5-cb0c-47fc-b303-4456a0d04880" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efe903cb1c03997b8902cfab651c05c0" ns3:_="" ns4:_="">
     <xsd:import namespace="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
@@ -893,22 +908,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="79f744f5-cb0c-47fc-b303-4456a0d04880"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30B054E4-AB9F-40CB-9C81-093D24B21832}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -925,29 +950,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="79f744f5-cb0c-47fc-b303-4456a0d04880"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Did the tests for Create, Owned and Puckemon. Fixed some bugs that they revealed.
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukas/Documents/GitHub/bEsTpRoGrAmMerS_EU/src/main/java/model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9F938B-CBF5-D047-9D81-AB070F70CD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59432C24-A591-4919-A936-6967348600A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2020" windowWidth="21600" windowHeight="11380" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
+    <workbookView xWindow="30735" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>Tackle,SwordsDance,Absorb</t>
   </si>
   <si>
-    <t>Tackle,SwordsDance,QuickAttack,DoubleEdge</t>
-  </si>
-  <si>
     <t>type/s</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Tackle</t>
+  </si>
+  <si>
+    <t>Tackle,SwordsDance,QuickAttack,DoubleEdge,Absorb</t>
   </si>
 </sst>
 </file>
@@ -468,22 +468,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB97F33-6489-4E92-9DBD-0E2293FD6E3B}">
   <dimension ref="A1:M129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K129" sqref="K129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" customWidth="1"/>
-    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -491,7 +491,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -521,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -529,7 +529,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>45</v>
@@ -553,7 +553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -561,7 +561,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>60</v>
@@ -585,7 +585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>80</v>
@@ -617,15 +617,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -646,10 +646,10 @@
         <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -657,7 +657,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -678,14 +678,14 @@
         <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L7" s="1"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -723,18 +723,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -909,6 +909,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB29C154-8763-432A-B38B-34E0AC157D49}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -921,14 +929,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="3b6923cc-94d7-4f86-8e31-1b1fa90ab430"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EA282A0-7F12-4AC5-A1E2-2835B8437EB5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added more JavaDoc. Cleaned up around the code. Added a reset method for Puckemon stats. They are now being reset after battles/switches. Fixed a bug with nickname.
</commit_message>
<xml_diff>
--- a/src/main/java/model/MonRegister.xlsx
+++ b/src/main/java/model/MonRegister.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\OneDrive\Dokument\GitHub\bEsTpRoGrAmMerS_EU\src\main\java\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59432C24-A591-4919-A936-6967348600A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7974EE9A-D050-4B2A-885D-070C020C8C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30735" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{D3FECC1C-64AA-4A3D-AE61-EF6A50938C94}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -42,9 +42,6 @@
     <t>move list</t>
   </si>
   <si>
-    <t>sprite list</t>
-  </si>
-  <si>
     <t>evolution lvl</t>
   </si>
   <si>
@@ -112,6 +109,18 @@
   </si>
   <si>
     <t>Tackle,SwordsDance,QuickAttack,DoubleEdge,Absorb</t>
+  </si>
+  <si>
+    <t>Lizardon</t>
+  </si>
+  <si>
+    <t>Explenation</t>
+  </si>
+  <si>
+    <t>If a puckemon cant evolve it should have evolution level 101 as it is unrechable and evolution id 0 as there is no Puckemon with that id</t>
+  </si>
+  <si>
+    <t>The excel checks for row id+1, so put the id on the right spot!</t>
   </si>
 </sst>
 </file>
@@ -466,70 +475,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB97F33-6489-4E92-9DBD-0E2293FD6E3B}">
-  <dimension ref="A1:M129"/>
+  <dimension ref="A1:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K129" sqref="K129"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="9" width="12.42578125" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
       <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
       </c>
       <c r="K1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
-        <v>2</v>
+      <c r="Q1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>45</v>
@@ -550,18 +560,21 @@
         <v>2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
         <v>60</v>
@@ -582,18 +595,21 @@
         <v>3</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>80</v>
@@ -614,18 +630,18 @@
         <v>0</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>40</v>
@@ -646,18 +662,18 @@
         <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>50</v>
@@ -672,17 +688,47 @@
         <v>50</v>
       </c>
       <c r="H6">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>78</v>
+      </c>
+      <c r="E7">
+        <v>84</v>
+      </c>
+      <c r="F7">
+        <v>78</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>101</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="L7" s="1"/>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
@@ -690,10 +736,10 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C129" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D129">
         <v>75</v>
@@ -714,7 +760,7 @@
         <v>0</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>